<commit_message>
Update latest forms and field mapping template
</commit_message>
<xml_diff>
--- a/clients/ArrowHead/content/entity/DealerPolicyFields.xlsx
+++ b/clients/ArrowHead/content/entity/DealerPolicyFields.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5430" uniqueCount="1844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5429" uniqueCount="1844">
   <si>
     <t xml:space="preserve">Field Name</t>
   </si>
@@ -3739,7 +3739,7 @@
     <t xml:space="preserve">number</t>
   </si>
   <si>
-    <t xml:space="preserve">Please enter the Ownership Percentage</t>
+    <t xml:space="preserve">Please enter valid Ownership Percentage</t>
   </si>
   <si>
     <t xml:space="preserve">antivirussoftware</t>
@@ -5565,7 +5565,7 @@
     <numFmt numFmtId="167" formatCode="0.00%"/>
     <numFmt numFmtId="168" formatCode="DD/MMM"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -5613,12 +5613,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -5659,7 +5653,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF9C0006"/>
+        <bgColor rgb="FF993300"/>
       </patternFill>
     </fill>
   </fills>
@@ -5739,7 +5733,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5852,10 +5846,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5868,7 +5858,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5904,7 +5894,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5916,7 +5906,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5930,6 +5920,17 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal 3" xfId="20"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+        <sz val="11"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -5940,7 +5941,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF9C0006"/>
+      <rgbColor rgb="FF800000"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -5971,7 +5972,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFC7CE"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF4472C4"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -6000,16 +6001,16 @@
   </sheetPr>
   <dimension ref="A1:S1529"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A685" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B697" activeCellId="0" sqref="B697"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A1014" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="P1026" activeCellId="0" sqref="P1026"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="18.0234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="45.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22980,7 +22981,7 @@
         <v>45</v>
       </c>
       <c r="K651" s="17"/>
-      <c r="L651" s="28" t="s">
+      <c r="L651" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M651" s="17"/>
@@ -23163,7 +23164,7 @@
         <v>45</v>
       </c>
       <c r="K658" s="17"/>
-      <c r="L658" s="28" t="s">
+      <c r="L658" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M658" s="17"/>
@@ -23346,7 +23347,7 @@
         <v>45</v>
       </c>
       <c r="K665" s="17"/>
-      <c r="L665" s="28" t="s">
+      <c r="L665" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M665" s="17"/>
@@ -24166,7 +24167,7 @@
         <v>45</v>
       </c>
       <c r="K697" s="17"/>
-      <c r="L697" s="28" t="s">
+      <c r="L697" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M697" s="17"/>
@@ -24349,7 +24350,7 @@
         <v>45</v>
       </c>
       <c r="K704" s="17"/>
-      <c r="L704" s="28" t="s">
+      <c r="L704" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M704" s="17"/>
@@ -24457,7 +24458,7 @@
         <v>45</v>
       </c>
       <c r="K708" s="17"/>
-      <c r="L708" s="28" t="s">
+      <c r="L708" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M708" s="17"/>
@@ -24640,7 +24641,7 @@
         <v>45</v>
       </c>
       <c r="K715" s="17"/>
-      <c r="L715" s="28" t="s">
+      <c r="L715" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M715" s="17"/>
@@ -24823,7 +24824,7 @@
         <v>45</v>
       </c>
       <c r="K722" s="17"/>
-      <c r="L722" s="28" t="s">
+      <c r="L722" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M722" s="17"/>
@@ -25217,7 +25218,7 @@
         <v>45</v>
       </c>
       <c r="K736" s="17"/>
-      <c r="L736" s="28" t="s">
+      <c r="L736" s="17" t="s">
         <v>637</v>
       </c>
       <c r="M736" s="17"/>
@@ -25969,7 +25970,7 @@
       <c r="G770" s="0" t="s">
         <v>964</v>
       </c>
-      <c r="I770" s="29"/>
+      <c r="I770" s="28"/>
     </row>
     <row r="771" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F771" s="0" t="s">
@@ -25997,29 +25998,29 @@
       </c>
     </row>
     <row r="773" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A773" s="29"/>
-      <c r="B773" s="29"/>
-      <c r="C773" s="29"/>
-      <c r="D773" s="29"/>
-      <c r="E773" s="29"/>
-      <c r="F773" s="29" t="s">
+      <c r="A773" s="28"/>
+      <c r="B773" s="28"/>
+      <c r="C773" s="28"/>
+      <c r="D773" s="28"/>
+      <c r="E773" s="28"/>
+      <c r="F773" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="G773" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H773" s="29"/>
-      <c r="J773" s="29"/>
-      <c r="K773" s="29"/>
-      <c r="L773" s="29"/>
-      <c r="M773" s="29"/>
-      <c r="N773" s="29"/>
-      <c r="O773" s="29"/>
-      <c r="P773" s="29"/>
-      <c r="Q773" s="29"/>
+      <c r="G773" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="H773" s="28"/>
+      <c r="J773" s="28"/>
+      <c r="K773" s="28"/>
+      <c r="L773" s="28"/>
+      <c r="M773" s="28"/>
+      <c r="N773" s="28"/>
+      <c r="O773" s="28"/>
+      <c r="P773" s="28"/>
+      <c r="Q773" s="28"/>
     </row>
     <row r="774" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B774" s="30"/>
+      <c r="B774" s="29"/>
       <c r="F774" s="0" t="s">
         <v>151</v>
       </c>
@@ -26219,7 +26220,7 @@
       </c>
     </row>
     <row r="791" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A791" s="29"/>
+      <c r="A791" s="28"/>
       <c r="F791" s="0" t="s">
         <v>159</v>
       </c>
@@ -26234,7 +26235,7 @@
       <c r="G792" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I792" s="29"/>
+      <c r="I792" s="28"/>
     </row>
     <row r="793" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A793" s="0" t="s">
@@ -26255,7 +26256,7 @@
       <c r="L793" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O793" s="31" t="s">
+      <c r="O793" s="30" t="s">
         <v>638</v>
       </c>
     </row>
@@ -26280,26 +26281,26 @@
       </c>
     </row>
     <row r="795" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A795" s="29"/>
-      <c r="B795" s="29"/>
-      <c r="C795" s="29"/>
-      <c r="D795" s="29"/>
-      <c r="E795" s="29"/>
-      <c r="F795" s="29" t="s">
+      <c r="A795" s="28"/>
+      <c r="B795" s="28"/>
+      <c r="C795" s="28"/>
+      <c r="D795" s="28"/>
+      <c r="E795" s="28"/>
+      <c r="F795" s="28" t="s">
         <v>986</v>
       </c>
-      <c r="G795" s="29" t="s">
+      <c r="G795" s="28" t="s">
         <v>987</v>
       </c>
-      <c r="H795" s="29"/>
-      <c r="J795" s="29"/>
-      <c r="K795" s="29"/>
-      <c r="L795" s="29"/>
-      <c r="M795" s="29"/>
-      <c r="N795" s="29"/>
-      <c r="O795" s="29"/>
-      <c r="P795" s="29"/>
-      <c r="Q795" s="29"/>
+      <c r="H795" s="28"/>
+      <c r="J795" s="28"/>
+      <c r="K795" s="28"/>
+      <c r="L795" s="28"/>
+      <c r="M795" s="28"/>
+      <c r="N795" s="28"/>
+      <c r="O795" s="28"/>
+      <c r="P795" s="28"/>
+      <c r="Q795" s="28"/>
     </row>
     <row r="796" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F796" s="0" t="s">
@@ -26326,7 +26327,7 @@
       </c>
     </row>
     <row r="799" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A799" s="29" t="s">
+      <c r="A799" s="28" t="s">
         <v>994</v>
       </c>
       <c r="B799" s="0" t="s">
@@ -26403,7 +26404,7 @@
       </c>
     </row>
     <row r="806" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A806" s="29"/>
+      <c r="A806" s="28"/>
       <c r="F806" s="0" t="s">
         <v>159</v>
       </c>
@@ -26470,7 +26471,7 @@
       </c>
     </row>
     <row r="812" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A812" s="29" t="s">
+      <c r="A812" s="28" t="s">
         <v>1004</v>
       </c>
       <c r="B812" s="0" t="s">
@@ -26521,7 +26522,7 @@
       <c r="L815" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O815" s="31" t="s">
+      <c r="O815" s="30" t="s">
         <v>638</v>
       </c>
     </row>
@@ -26551,7 +26552,7 @@
       </c>
     </row>
     <row r="818" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A818" s="29"/>
+      <c r="A818" s="28"/>
       <c r="F818" s="0" t="s">
         <v>151</v>
       </c>
@@ -26963,7 +26964,7 @@
       <c r="E857" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H857" s="32"/>
+      <c r="H857" s="31"/>
       <c r="J857" s="0" t="s">
         <v>21</v>
       </c>
@@ -26975,13 +26976,13 @@
       <c r="G858" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H858" s="32"/>
+      <c r="H858" s="31"/>
     </row>
     <row r="859" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F859" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G859" s="33" t="s">
+      <c r="G859" s="32" t="s">
         <v>45</v>
       </c>
     </row>
@@ -26998,7 +26999,7 @@
       <c r="E860" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G860" s="33"/>
+      <c r="G860" s="32"/>
       <c r="J860" s="0" t="s">
         <v>21</v>
       </c>
@@ -27007,7 +27008,7 @@
       <c r="F861" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G861" s="33" t="s">
+      <c r="G861" s="32" t="s">
         <v>21</v>
       </c>
     </row>
@@ -27015,7 +27016,7 @@
       <c r="F862" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G862" s="33" t="s">
+      <c r="G862" s="32" t="s">
         <v>45</v>
       </c>
     </row>
@@ -27032,7 +27033,7 @@
       <c r="E863" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G863" s="33"/>
+      <c r="G863" s="32"/>
       <c r="J863" s="0" t="s">
         <v>21</v>
       </c>
@@ -27041,7 +27042,7 @@
       <c r="F864" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G864" s="33" t="s">
+      <c r="G864" s="32" t="s">
         <v>21</v>
       </c>
     </row>
@@ -27049,7 +27050,7 @@
       <c r="F865" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G865" s="33" t="s">
+      <c r="G865" s="32" t="s">
         <v>45</v>
       </c>
     </row>
@@ -27066,7 +27067,7 @@
       <c r="E866" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G866" s="33"/>
+      <c r="G866" s="32"/>
       <c r="H866" s="0" t="s">
         <v>1056</v>
       </c>
@@ -27087,7 +27088,7 @@
       <c r="E867" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G867" s="33"/>
+      <c r="G867" s="32"/>
       <c r="J867" s="0" t="s">
         <v>21</v>
       </c>
@@ -27096,7 +27097,7 @@
       <c r="F868" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G868" s="33" t="s">
+      <c r="G868" s="32" t="s">
         <v>21</v>
       </c>
     </row>
@@ -27104,7 +27105,7 @@
       <c r="F869" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G869" s="33" t="s">
+      <c r="G869" s="32" t="s">
         <v>45</v>
       </c>
     </row>
@@ -27121,7 +27122,7 @@
       <c r="E870" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G870" s="33"/>
+      <c r="G870" s="32"/>
       <c r="H870" s="0" t="s">
         <v>1056</v>
       </c>
@@ -27142,7 +27143,7 @@
       <c r="E871" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G871" s="33"/>
+      <c r="G871" s="32"/>
       <c r="J871" s="0" t="s">
         <v>21</v>
       </c>
@@ -27176,7 +27177,7 @@
       <c r="E874" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G874" s="34"/>
+      <c r="G874" s="33"/>
       <c r="H874" s="0" t="s">
         <v>1064</v>
       </c>
@@ -27197,7 +27198,7 @@
       <c r="E875" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="G875" s="34"/>
+      <c r="G875" s="33"/>
       <c r="H875" s="0" t="s">
         <v>24</v>
       </c>
@@ -27221,7 +27222,7 @@
       <c r="E876" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G876" s="34"/>
+      <c r="G876" s="33"/>
       <c r="H876" s="0" t="s">
         <v>1068</v>
       </c>
@@ -27242,7 +27243,7 @@
       <c r="E877" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G877" s="34"/>
+      <c r="G877" s="33"/>
       <c r="H877" s="0" t="s">
         <v>1071</v>
       </c>
@@ -27254,7 +27255,7 @@
       <c r="F878" s="0" t="s">
         <v>1072</v>
       </c>
-      <c r="G878" s="34" t="s">
+      <c r="G878" s="33" t="s">
         <v>1073</v>
       </c>
     </row>
@@ -27262,7 +27263,7 @@
       <c r="F879" s="0" t="s">
         <v>1074</v>
       </c>
-      <c r="G879" s="34" t="s">
+      <c r="G879" s="33" t="s">
         <v>1075</v>
       </c>
     </row>
@@ -27270,7 +27271,7 @@
       <c r="F880" s="0" t="s">
         <v>1076</v>
       </c>
-      <c r="G880" s="33" t="s">
+      <c r="G880" s="32" t="s">
         <v>1077</v>
       </c>
     </row>
@@ -27278,7 +27279,7 @@
       <c r="F881" s="0" t="s">
         <v>1078</v>
       </c>
-      <c r="G881" s="33" t="s">
+      <c r="G881" s="32" t="s">
         <v>1079</v>
       </c>
     </row>
@@ -27286,7 +27287,7 @@
       <c r="F882" s="0" t="s">
         <v>1080</v>
       </c>
-      <c r="G882" s="33" t="s">
+      <c r="G882" s="32" t="s">
         <v>1081</v>
       </c>
     </row>
@@ -27294,7 +27295,7 @@
       <c r="F883" s="0" t="s">
         <v>1082</v>
       </c>
-      <c r="G883" s="33" t="s">
+      <c r="G883" s="32" t="s">
         <v>1083</v>
       </c>
     </row>
@@ -27302,7 +27303,7 @@
       <c r="F884" s="0" t="s">
         <v>1084</v>
       </c>
-      <c r="G884" s="33" t="s">
+      <c r="G884" s="32" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -27310,7 +27311,7 @@
       <c r="F885" s="0" t="s">
         <v>1086</v>
       </c>
-      <c r="G885" s="33" t="s">
+      <c r="G885" s="32" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -27318,7 +27319,7 @@
       <c r="F886" s="0" t="s">
         <v>1088</v>
       </c>
-      <c r="G886" s="33" t="s">
+      <c r="G886" s="32" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -27326,31 +27327,31 @@
       <c r="F887" s="0" t="s">
         <v>1090</v>
       </c>
-      <c r="G887" s="33" t="s">
+      <c r="G887" s="32" t="s">
         <v>1091</v>
       </c>
     </row>
     <row r="888" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A888" s="29"/>
-      <c r="B888" s="29"/>
-      <c r="C888" s="29"/>
-      <c r="D888" s="29"/>
-      <c r="E888" s="29"/>
-      <c r="F888" s="29" t="s">
+      <c r="A888" s="28"/>
+      <c r="B888" s="28"/>
+      <c r="C888" s="28"/>
+      <c r="D888" s="28"/>
+      <c r="E888" s="28"/>
+      <c r="F888" s="28" t="s">
         <v>1092</v>
       </c>
-      <c r="G888" s="29" t="s">
+      <c r="G888" s="28" t="s">
         <v>1093</v>
       </c>
-      <c r="H888" s="29"/>
-      <c r="J888" s="29"/>
-      <c r="K888" s="29"/>
-      <c r="L888" s="29"/>
-      <c r="M888" s="29"/>
-      <c r="N888" s="29"/>
-      <c r="O888" s="29"/>
-      <c r="P888" s="29"/>
-      <c r="Q888" s="29"/>
+      <c r="H888" s="28"/>
+      <c r="J888" s="28"/>
+      <c r="K888" s="28"/>
+      <c r="L888" s="28"/>
+      <c r="M888" s="28"/>
+      <c r="N888" s="28"/>
+      <c r="O888" s="28"/>
+      <c r="P888" s="28"/>
+      <c r="Q888" s="28"/>
     </row>
     <row r="889" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F889" s="0" t="s">
@@ -27364,7 +27365,7 @@
       <c r="F890" s="0" t="s">
         <v>1096</v>
       </c>
-      <c r="G890" s="35" t="s">
+      <c r="G890" s="34" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -27381,7 +27382,7 @@
       <c r="E891" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G891" s="35"/>
+      <c r="G891" s="34"/>
       <c r="H891" s="0" t="s">
         <v>1071</v>
       </c>
@@ -27390,53 +27391,53 @@
       </c>
     </row>
     <row r="892" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F892" s="36" t="s">
+      <c r="F892" s="35" t="s">
         <v>1100</v>
       </c>
-      <c r="G892" s="35" t="s">
+      <c r="G892" s="34" t="s">
         <v>1101</v>
       </c>
     </row>
     <row r="893" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F893" s="36" t="s">
+      <c r="F893" s="35" t="s">
         <v>406</v>
       </c>
-      <c r="G893" s="35" t="s">
+      <c r="G893" s="34" t="s">
         <v>1102</v>
       </c>
     </row>
     <row r="894" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F894" s="36" t="s">
+      <c r="F894" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="G894" s="35" t="s">
+      <c r="G894" s="34" t="s">
         <v>358</v>
       </c>
     </row>
     <row r="895" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A895" s="29"/>
-      <c r="B895" s="29"/>
-      <c r="C895" s="29"/>
-      <c r="D895" s="29"/>
-      <c r="E895" s="29"/>
-      <c r="F895" s="29" t="s">
+      <c r="A895" s="28"/>
+      <c r="B895" s="28"/>
+      <c r="C895" s="28"/>
+      <c r="D895" s="28"/>
+      <c r="E895" s="28"/>
+      <c r="F895" s="28" t="s">
         <v>1103</v>
       </c>
-      <c r="G895" s="29" t="s">
+      <c r="G895" s="28" t="s">
         <v>1104</v>
       </c>
-      <c r="H895" s="29"/>
-      <c r="J895" s="29"/>
-      <c r="K895" s="29"/>
-      <c r="L895" s="29"/>
-      <c r="M895" s="29"/>
-      <c r="N895" s="29"/>
-      <c r="O895" s="29"/>
-      <c r="P895" s="29"/>
-      <c r="Q895" s="29"/>
+      <c r="H895" s="28"/>
+      <c r="J895" s="28"/>
+      <c r="K895" s="28"/>
+      <c r="L895" s="28"/>
+      <c r="M895" s="28"/>
+      <c r="N895" s="28"/>
+      <c r="O895" s="28"/>
+      <c r="P895" s="28"/>
+      <c r="Q895" s="28"/>
     </row>
     <row r="896" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F896" s="36" t="s">
+      <c r="F896" s="35" t="s">
         <v>359</v>
       </c>
       <c r="G896" s="0" t="s">
@@ -27444,55 +27445,55 @@
       </c>
     </row>
     <row r="897" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F897" s="36" t="s">
+      <c r="F897" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="G897" s="35" t="s">
+      <c r="G897" s="34" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="898" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F898" s="36" t="s">
+      <c r="F898" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="G898" s="35" t="s">
+      <c r="G898" s="34" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="899" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F899" s="36" t="s">
+      <c r="F899" s="35" t="s">
         <v>1074</v>
       </c>
-      <c r="G899" s="35" t="s">
+      <c r="G899" s="34" t="s">
         <v>1075</v>
       </c>
     </row>
     <row r="900" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F900" s="36" t="s">
+      <c r="F900" s="35" t="s">
         <v>1078</v>
       </c>
-      <c r="G900" s="35" t="s">
+      <c r="G900" s="34" t="s">
         <v>1079</v>
       </c>
     </row>
     <row r="901" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F901" s="36" t="s">
+      <c r="F901" s="35" t="s">
         <v>1084</v>
       </c>
-      <c r="G901" s="35" t="s">
+      <c r="G901" s="34" t="s">
         <v>1085</v>
       </c>
     </row>
     <row r="902" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F902" s="36" t="s">
+      <c r="F902" s="35" t="s">
         <v>1088</v>
       </c>
-      <c r="G902" s="35" t="s">
+      <c r="G902" s="34" t="s">
         <v>1089</v>
       </c>
     </row>
     <row r="903" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F903" s="36" t="s">
+      <c r="F903" s="35" t="s">
         <v>1090</v>
       </c>
       <c r="G903" s="0" t="s">
@@ -27500,7 +27501,7 @@
       </c>
     </row>
     <row r="904" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F904" s="36" t="s">
+      <c r="F904" s="35" t="s">
         <v>1092</v>
       </c>
       <c r="G904" s="0" t="s">
@@ -27508,18 +27509,18 @@
       </c>
     </row>
     <row r="905" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F905" s="36" t="s">
+      <c r="F905" s="35" t="s">
         <v>1094</v>
       </c>
-      <c r="G905" s="34" t="s">
+      <c r="G905" s="33" t="s">
         <v>1095</v>
       </c>
     </row>
     <row r="906" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="F906" s="36" t="s">
+      <c r="F906" s="35" t="s">
         <v>1096</v>
       </c>
-      <c r="G906" s="34" t="s">
+      <c r="G906" s="33" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -27536,7 +27537,7 @@
       <c r="E907" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G907" s="34"/>
+      <c r="G907" s="33"/>
       <c r="H907" s="0" t="s">
         <v>1071</v>
       </c>
@@ -27548,7 +27549,7 @@
       <c r="F908" s="0" t="s">
         <v>1107</v>
       </c>
-      <c r="G908" s="34" t="s">
+      <c r="G908" s="33" t="s">
         <v>1108</v>
       </c>
     </row>
@@ -27556,7 +27557,7 @@
       <c r="F909" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="G909" s="34" t="s">
+      <c r="G909" s="33" t="s">
         <v>486</v>
       </c>
     </row>
@@ -27564,7 +27565,7 @@
       <c r="F910" s="0" t="s">
         <v>1109</v>
       </c>
-      <c r="G910" s="34" t="s">
+      <c r="G910" s="33" t="s">
         <v>1110</v>
       </c>
     </row>
@@ -27572,7 +27573,7 @@
       <c r="F911" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="G911" s="34" t="s">
+      <c r="G911" s="33" t="s">
         <v>352</v>
       </c>
     </row>
@@ -27605,7 +27606,7 @@
       <c r="E914" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G914" s="34"/>
+      <c r="G914" s="33"/>
       <c r="H914" s="0" t="s">
         <v>1071</v>
       </c>
@@ -27617,7 +27618,7 @@
       <c r="F915" s="0" t="s">
         <v>1107</v>
       </c>
-      <c r="G915" s="34" t="s">
+      <c r="G915" s="33" t="s">
         <v>1108</v>
       </c>
     </row>
@@ -27625,7 +27626,7 @@
       <c r="F916" s="0" t="s">
         <v>485</v>
       </c>
-      <c r="G916" s="34" t="s">
+      <c r="G916" s="33" t="s">
         <v>486</v>
       </c>
     </row>
@@ -27633,7 +27634,7 @@
       <c r="F917" s="0" t="s">
         <v>351</v>
       </c>
-      <c r="G917" s="34" t="s">
+      <c r="G917" s="33" t="s">
         <v>352</v>
       </c>
     </row>
@@ -27641,7 +27642,7 @@
       <c r="F918" s="0" t="s">
         <v>353</v>
       </c>
-      <c r="G918" s="34" t="s">
+      <c r="G918" s="33" t="s">
         <v>354</v>
       </c>
     </row>
@@ -27658,11 +27659,11 @@
       <c r="E919" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G919" s="34"/>
+      <c r="G919" s="33"/>
       <c r="H919" s="0" t="s">
         <v>1071</v>
       </c>
-      <c r="I919" s="34"/>
+      <c r="I919" s="33"/>
       <c r="J919" s="0" t="s">
         <v>45</v>
       </c>
@@ -27674,7 +27675,7 @@
       <c r="G920" s="0" t="s">
         <v>1101</v>
       </c>
-      <c r="I920" s="34"/>
+      <c r="I920" s="33"/>
     </row>
     <row r="921" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F921" s="0" t="s">
@@ -27683,8 +27684,8 @@
       <c r="G921" s="0" t="s">
         <v>358</v>
       </c>
-      <c r="H921" s="32"/>
-      <c r="I921" s="34"/>
+      <c r="H921" s="31"/>
+      <c r="I921" s="33"/>
     </row>
     <row r="922" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F922" s="0" t="s">
@@ -27693,7 +27694,7 @@
       <c r="G922" s="0" t="s">
         <v>1118</v>
       </c>
-      <c r="H922" s="32"/>
+      <c r="H922" s="31"/>
     </row>
     <row r="923" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F923" s="0" t="s">
@@ -27702,7 +27703,7 @@
       <c r="G923" s="0" t="s">
         <v>1104</v>
       </c>
-      <c r="H923" s="32"/>
+      <c r="H923" s="31"/>
     </row>
     <row r="924" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F924" s="0" t="s">
@@ -27711,7 +27712,7 @@
       <c r="G924" s="0" t="s">
         <v>1120</v>
       </c>
-      <c r="H924" s="32"/>
+      <c r="H924" s="31"/>
     </row>
     <row r="925" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F925" s="0" t="s">
@@ -27753,7 +27754,7 @@
       <c r="H928" s="0" t="s">
         <v>1071</v>
       </c>
-      <c r="I928" s="36"/>
+      <c r="I928" s="35"/>
       <c r="J928" s="0" t="s">
         <v>45</v>
       </c>
@@ -27902,7 +27903,7 @@
       <c r="A942" s="0" t="s">
         <v>1130</v>
       </c>
-      <c r="B942" s="37" t="s">
+      <c r="B942" s="36" t="s">
         <v>1131</v>
       </c>
       <c r="C942" s="0" t="s">
@@ -27965,7 +27966,7 @@
       </c>
     </row>
     <row r="948" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A948" s="38" t="s">
+      <c r="A948" s="37" t="s">
         <v>1142</v>
       </c>
       <c r="B948" s="0" t="s">
@@ -28009,7 +28010,7 @@
       </c>
     </row>
     <row r="952" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A952" s="38" t="s">
+      <c r="A952" s="37" t="s">
         <v>1150</v>
       </c>
       <c r="B952" s="0" t="s">
@@ -28053,7 +28054,7 @@
       </c>
     </row>
     <row r="956" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A956" s="38" t="s">
+      <c r="A956" s="37" t="s">
         <v>1158</v>
       </c>
       <c r="B956" s="0" t="s">
@@ -28097,7 +28098,7 @@
       </c>
     </row>
     <row r="960" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A960" s="38" t="s">
+      <c r="A960" s="37" t="s">
         <v>1166</v>
       </c>
       <c r="B960" s="0" t="s">
@@ -28141,7 +28142,7 @@
       </c>
     </row>
     <row r="964" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A964" s="38" t="s">
+      <c r="A964" s="37" t="s">
         <v>1132</v>
       </c>
       <c r="B964" s="0" t="s">
@@ -28185,7 +28186,7 @@
       </c>
     </row>
     <row r="968" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A968" s="38" t="s">
+      <c r="A968" s="37" t="s">
         <v>1138</v>
       </c>
       <c r="B968" s="0" t="s">
@@ -28682,15 +28683,15 @@
       </c>
     </row>
     <row r="1008" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1008" s="39"/>
-      <c r="B1008" s="39"/>
+      <c r="A1008" s="38"/>
+      <c r="B1008" s="38"/>
       <c r="F1008" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1008" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1008" s="39"/>
+      <c r="H1008" s="38"/>
     </row>
     <row r="1009" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1009" s="0" t="s">
@@ -28721,10 +28722,10 @@
       </c>
     </row>
     <row r="1011" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1011" s="39" t="s">
+      <c r="A1011" s="38" t="s">
         <v>1207</v>
       </c>
-      <c r="B1011" s="39" t="s">
+      <c r="B1011" s="38" t="s">
         <v>1208</v>
       </c>
       <c r="D1011" s="0" t="s">
@@ -28733,7 +28734,7 @@
       <c r="E1011" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1011" s="39" t="s">
+      <c r="H1011" s="38" t="s">
         <v>1208</v>
       </c>
       <c r="J1011" s="0" t="s">
@@ -28781,10 +28782,10 @@
       </c>
     </row>
     <row r="1014" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1014" s="39" t="s">
+      <c r="A1014" s="38" t="s">
         <v>1213</v>
       </c>
-      <c r="B1014" s="39" t="s">
+      <c r="B1014" s="38" t="s">
         <v>1214</v>
       </c>
       <c r="D1014" s="0" t="s">
@@ -28793,7 +28794,7 @@
       <c r="E1014" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1014" s="39" t="s">
+      <c r="H1014" s="38" t="s">
         <v>1214</v>
       </c>
       <c r="J1014" s="0" t="s">
@@ -28841,10 +28842,10 @@
       </c>
     </row>
     <row r="1017" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1017" s="39" t="s">
+      <c r="A1017" s="38" t="s">
         <v>1219</v>
       </c>
-      <c r="B1017" s="39" t="s">
+      <c r="B1017" s="38" t="s">
         <v>1220</v>
       </c>
       <c r="D1017" s="0" t="s">
@@ -28853,7 +28854,7 @@
       <c r="E1017" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1017" s="39" t="s">
+      <c r="H1017" s="38" t="s">
         <v>1220</v>
       </c>
       <c r="J1017" s="0" t="s">
@@ -28901,10 +28902,10 @@
       </c>
     </row>
     <row r="1020" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1020" s="39" t="s">
+      <c r="A1020" s="38" t="s">
         <v>1225</v>
       </c>
-      <c r="B1020" s="39" t="s">
+      <c r="B1020" s="38" t="s">
         <v>1226</v>
       </c>
       <c r="D1020" s="5" t="s">
@@ -28913,7 +28914,7 @@
       <c r="E1020" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1020" s="39" t="s">
+      <c r="H1020" s="38" t="s">
         <v>1226</v>
       </c>
       <c r="J1020" s="0" t="s">
@@ -28924,16 +28925,16 @@
       <c r="A1021" s="0" t="s">
         <v>1227</v>
       </c>
-      <c r="B1021" s="39" t="s">
+      <c r="B1021" s="38" t="s">
         <v>1228</v>
       </c>
-      <c r="D1021" s="40" t="s">
+      <c r="D1021" s="39" t="s">
         <v>63</v>
       </c>
       <c r="E1021" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1021" s="39" t="s">
+      <c r="H1021" s="38" t="s">
         <v>1228</v>
       </c>
       <c r="J1021" s="0" t="s">
@@ -28941,19 +28942,19 @@
       </c>
     </row>
     <row r="1022" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1022" s="39" t="s">
+      <c r="A1022" s="38" t="s">
         <v>1229</v>
       </c>
-      <c r="B1022" s="39" t="s">
+      <c r="B1022" s="38" t="s">
         <v>1230</v>
       </c>
-      <c r="D1022" s="41" t="s">
+      <c r="D1022" s="40" t="s">
         <v>63</v>
       </c>
       <c r="E1022" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1022" s="39" t="s">
+      <c r="H1022" s="38" t="s">
         <v>1230</v>
       </c>
       <c r="J1022" s="0" t="s">
@@ -28964,7 +28965,7 @@
       <c r="A1023" s="0" t="s">
         <v>1231</v>
       </c>
-      <c r="B1023" s="39" t="s">
+      <c r="B1023" s="38" t="s">
         <v>914</v>
       </c>
       <c r="D1023" s="5" t="s">
@@ -28973,7 +28974,7 @@
       <c r="E1023" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1023" s="39" t="s">
+      <c r="H1023" s="38" t="s">
         <v>914</v>
       </c>
       <c r="J1023" s="0" t="s">
@@ -28984,22 +28985,22 @@
       <c r="A1024" s="0" t="s">
         <v>1232</v>
       </c>
-      <c r="B1024" s="39" t="s">
+      <c r="B1024" s="38" t="s">
         <v>1233</v>
       </c>
       <c r="D1024" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="E1024" s="42" t="s">
+      <c r="E1024" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="H1024" s="39"/>
+      <c r="H1024" s="38"/>
     </row>
     <row r="1025" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1025" s="0" t="s">
         <v>1234</v>
       </c>
-      <c r="B1025" s="39" t="s">
+      <c r="B1025" s="38" t="s">
         <v>304</v>
       </c>
       <c r="C1025" s="0" t="s">
@@ -29011,7 +29012,7 @@
       <c r="E1025" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1025" s="39" t="s">
+      <c r="H1025" s="38" t="s">
         <v>304</v>
       </c>
       <c r="J1025" s="0" t="s">
@@ -29025,7 +29026,7 @@
       <c r="A1026" s="0" t="s">
         <v>1236</v>
       </c>
-      <c r="B1026" s="39" t="s">
+      <c r="B1026" s="38" t="s">
         <v>1237</v>
       </c>
       <c r="C1026" s="0" t="s">
@@ -29037,7 +29038,7 @@
       <c r="E1026" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H1026" s="39" t="s">
+      <c r="H1026" s="38" t="s">
         <v>1237</v>
       </c>
       <c r="J1026" s="0" t="s">
@@ -29057,7 +29058,7 @@
       <c r="A1027" s="0" t="s">
         <v>1240</v>
       </c>
-      <c r="B1027" s="39" t="s">
+      <c r="B1027" s="38" t="s">
         <v>1241</v>
       </c>
       <c r="D1027" s="0" t="s">
@@ -29066,7 +29067,7 @@
       <c r="E1027" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1027" s="39"/>
+      <c r="H1027" s="38"/>
       <c r="J1027" s="0" t="s">
         <v>45</v>
       </c>
@@ -29105,14 +29106,14 @@
       </c>
     </row>
     <row r="1031" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1031" s="39"/>
+      <c r="B1031" s="38"/>
       <c r="F1031" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1031" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1031" s="39"/>
+      <c r="H1031" s="38"/>
     </row>
     <row r="1032" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1032" s="0" t="s">
@@ -29219,7 +29220,7 @@
       <c r="A1040" s="0" t="s">
         <v>1251</v>
       </c>
-      <c r="B1040" s="39" t="s">
+      <c r="B1040" s="38" t="s">
         <v>1252</v>
       </c>
       <c r="D1040" s="0" t="s">
@@ -29228,7 +29229,7 @@
       <c r="E1040" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1040" s="39" t="s">
+      <c r="H1040" s="38" t="s">
         <v>1253</v>
       </c>
       <c r="J1040" s="0" t="s">
@@ -29279,7 +29280,7 @@
       <c r="A1043" s="0" t="s">
         <v>1259</v>
       </c>
-      <c r="B1043" s="39" t="s">
+      <c r="B1043" s="38" t="s">
         <v>1260</v>
       </c>
       <c r="D1043" s="0" t="s">
@@ -29288,7 +29289,7 @@
       <c r="E1043" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1043" s="39" t="s">
+      <c r="H1043" s="38" t="s">
         <v>1261</v>
       </c>
       <c r="J1043" s="0" t="s">
@@ -29333,14 +29334,14 @@
       </c>
     </row>
     <row r="1046" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1046" s="39"/>
+      <c r="B1046" s="38"/>
       <c r="F1046" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1046" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1046" s="39"/>
+      <c r="H1046" s="38"/>
     </row>
     <row r="1047" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1047" s="0" t="s">
@@ -29374,7 +29375,7 @@
       <c r="A1049" s="0" t="s">
         <v>1270</v>
       </c>
-      <c r="B1049" s="39" t="s">
+      <c r="B1049" s="38" t="s">
         <v>1271</v>
       </c>
       <c r="D1049" s="5" t="s">
@@ -29383,20 +29384,20 @@
       <c r="E1049" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1049" s="39"/>
+      <c r="H1049" s="38"/>
       <c r="J1049" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="1050" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1050" s="39"/>
+      <c r="B1050" s="38"/>
       <c r="F1050" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1050" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1050" s="39"/>
+      <c r="H1050" s="38"/>
     </row>
     <row r="1051" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1051" s="0" t="s">
@@ -29430,7 +29431,7 @@
       <c r="A1053" s="0" t="s">
         <v>1273</v>
       </c>
-      <c r="B1053" s="39" t="s">
+      <c r="B1053" s="38" t="s">
         <v>914</v>
       </c>
       <c r="D1053" s="0" t="s">
@@ -29439,7 +29440,7 @@
       <c r="E1053" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1053" s="39" t="s">
+      <c r="H1053" s="38" t="s">
         <v>914</v>
       </c>
       <c r="J1053" s="0" t="s">
@@ -29490,7 +29491,7 @@
       <c r="A1056" s="0" t="s">
         <v>1276</v>
       </c>
-      <c r="B1056" s="39" t="s">
+      <c r="B1056" s="38" t="s">
         <v>1277</v>
       </c>
       <c r="D1056" s="0" t="s">
@@ -29499,7 +29500,7 @@
       <c r="E1056" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="H1056" s="39" t="s">
+      <c r="H1056" s="38" t="s">
         <v>24</v>
       </c>
       <c r="J1056" s="0" t="s">
@@ -29550,14 +29551,14 @@
       </c>
     </row>
     <row r="1059" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1059" s="39"/>
+      <c r="B1059" s="38"/>
       <c r="F1059" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1059" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1059" s="39"/>
+      <c r="H1059" s="38"/>
     </row>
     <row r="1060" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1060" s="0" t="s">
@@ -29585,7 +29586,7 @@
       </c>
     </row>
     <row r="1062" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1062" s="39"/>
+      <c r="B1062" s="38"/>
       <c r="D1062" s="5"/>
       <c r="E1062" s="5"/>
       <c r="F1062" s="0" t="s">
@@ -29594,10 +29595,10 @@
       <c r="G1062" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1062" s="39"/>
+      <c r="H1062" s="38"/>
     </row>
     <row r="1063" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1063" s="39"/>
+      <c r="B1063" s="38"/>
       <c r="D1063" s="5"/>
       <c r="E1063" s="5"/>
       <c r="F1063" s="0" t="s">
@@ -29606,62 +29607,62 @@
       <c r="G1063" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1063" s="39"/>
+      <c r="H1063" s="38"/>
     </row>
     <row r="1064" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1064" s="0" t="s">
         <v>1283</v>
       </c>
-      <c r="B1064" s="39" t="s">
+      <c r="B1064" s="38" t="s">
         <v>1284</v>
       </c>
       <c r="D1064" s="0" t="s">
         <v>612</v>
       </c>
-      <c r="E1064" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1064" s="39"/>
+      <c r="E1064" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1064" s="38"/>
       <c r="J1064" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="1065" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1065" s="39"/>
-      <c r="E1065" s="36"/>
+      <c r="B1065" s="38"/>
+      <c r="E1065" s="35"/>
       <c r="F1065" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1065" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1065" s="39"/>
+      <c r="H1065" s="38"/>
     </row>
     <row r="1066" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1066" s="39"/>
-      <c r="E1066" s="36"/>
+      <c r="B1066" s="38"/>
+      <c r="E1066" s="35"/>
       <c r="F1066" s="0" t="s">
         <v>151</v>
       </c>
       <c r="G1066" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1066" s="39"/>
+      <c r="H1066" s="38"/>
     </row>
     <row r="1067" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1067" s="0" t="s">
         <v>1285</v>
       </c>
-      <c r="B1067" s="39" t="s">
+      <c r="B1067" s="38" t="s">
         <v>1286</v>
       </c>
       <c r="D1067" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E1067" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1067" s="39" t="s">
+      <c r="E1067" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1067" s="38" t="s">
         <v>1287</v>
       </c>
       <c r="J1067" s="0" t="s">
@@ -29672,7 +29673,7 @@
       <c r="A1068" s="0" t="s">
         <v>1288</v>
       </c>
-      <c r="B1068" s="39" t="s">
+      <c r="B1068" s="38" t="s">
         <v>1289</v>
       </c>
       <c r="D1068" s="0" t="s">
@@ -29681,7 +29682,7 @@
       <c r="E1068" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1068" s="39"/>
+      <c r="H1068" s="38"/>
       <c r="J1068" s="0" t="s">
         <v>45</v>
       </c>
@@ -29706,7 +29707,7 @@
       <c r="A1071" s="0" t="s">
         <v>1290</v>
       </c>
-      <c r="B1071" s="39" t="s">
+      <c r="B1071" s="38" t="s">
         <v>1291</v>
       </c>
       <c r="D1071" s="0" t="s">
@@ -29715,7 +29716,7 @@
       <c r="E1071" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1071" s="39"/>
+      <c r="H1071" s="38"/>
       <c r="J1071" s="0" t="s">
         <v>45</v>
       </c>
@@ -29740,7 +29741,7 @@
       <c r="A1074" s="0" t="s">
         <v>1292</v>
       </c>
-      <c r="B1074" s="39" t="s">
+      <c r="B1074" s="38" t="s">
         <v>1293</v>
       </c>
       <c r="D1074" s="0" t="s">
@@ -29749,7 +29750,7 @@
       <c r="E1074" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1074" s="39"/>
+      <c r="H1074" s="38"/>
       <c r="J1074" s="0" t="s">
         <v>45</v>
       </c>
@@ -29774,7 +29775,7 @@
       <c r="A1077" s="0" t="s">
         <v>1294</v>
       </c>
-      <c r="B1077" s="39" t="s">
+      <c r="B1077" s="38" t="s">
         <v>1295</v>
       </c>
       <c r="D1077" s="5" t="s">
@@ -29783,13 +29784,13 @@
       <c r="E1077" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H1077" s="39"/>
+      <c r="H1077" s="38"/>
       <c r="J1077" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="1078" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1078" s="39"/>
+      <c r="B1078" s="38"/>
       <c r="D1078" s="5"/>
       <c r="E1078" s="5"/>
       <c r="F1078" s="0" t="s">
@@ -29798,33 +29799,33 @@
       <c r="G1078" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1078" s="39"/>
+      <c r="H1078" s="38"/>
     </row>
     <row r="1079" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1079" s="39"/>
-      <c r="E1079" s="36"/>
+      <c r="B1079" s="38"/>
+      <c r="E1079" s="35"/>
       <c r="F1079" s="0" t="s">
         <v>151</v>
       </c>
       <c r="G1079" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1079" s="39"/>
+      <c r="H1079" s="38"/>
     </row>
     <row r="1080" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1080" s="0" t="s">
         <v>1296</v>
       </c>
-      <c r="B1080" s="39" t="s">
+      <c r="B1080" s="38" t="s">
         <v>1297</v>
       </c>
       <c r="D1080" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E1080" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1080" s="39" t="s">
+      <c r="E1080" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1080" s="38" t="s">
         <v>1298</v>
       </c>
       <c r="J1080" s="0" t="s">
@@ -29835,31 +29836,29 @@
       <c r="A1081" s="0" t="s">
         <v>1299</v>
       </c>
-      <c r="B1081" s="39" t="s">
+      <c r="B1081" s="38" t="s">
         <v>1300</v>
       </c>
       <c r="D1081" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1081" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1081" s="39" t="s">
-        <v>34</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="E1081" s="35" t="s">
+        <v>300</v>
+      </c>
+      <c r="H1081" s="38"/>
       <c r="J1081" s="0" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="1082" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1082" s="39"/>
+      <c r="B1082" s="38"/>
       <c r="F1082" s="0" t="s">
         <v>1301</v>
       </c>
       <c r="G1082" s="0" t="s">
         <v>1302</v>
       </c>
-      <c r="H1082" s="39"/>
+      <c r="H1082" s="38"/>
     </row>
     <row r="1083" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1083" s="0" t="s">
@@ -29881,7 +29880,7 @@
       <c r="A1085" s="0" t="s">
         <v>1307</v>
       </c>
-      <c r="B1085" s="39" t="s">
+      <c r="B1085" s="38" t="s">
         <v>1308</v>
       </c>
       <c r="D1085" s="0" t="s">
@@ -29890,7 +29889,7 @@
       <c r="E1085" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1085" s="39" t="s">
+      <c r="H1085" s="38" t="s">
         <v>1309</v>
       </c>
       <c r="J1085" s="0" t="s">
@@ -29923,14 +29922,14 @@
       </c>
     </row>
     <row r="1088" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1088" s="39"/>
+      <c r="B1088" s="38"/>
       <c r="F1088" s="0" t="s">
         <v>151</v>
       </c>
       <c r="G1088" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1088" s="39"/>
+      <c r="H1088" s="38"/>
     </row>
     <row r="1089" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1089" s="0" t="s">
@@ -29958,14 +29957,14 @@
       </c>
     </row>
     <row r="1091" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1091" s="39"/>
+      <c r="B1091" s="38"/>
       <c r="F1091" s="0" t="s">
         <v>151</v>
       </c>
       <c r="G1091" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1091" s="39"/>
+      <c r="H1091" s="38"/>
     </row>
     <row r="1092" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1092" s="0" t="s">
@@ -29993,15 +29992,15 @@
       </c>
     </row>
     <row r="1094" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1094" s="39"/>
-      <c r="B1094" s="39"/>
+      <c r="A1094" s="38"/>
+      <c r="B1094" s="38"/>
       <c r="F1094" s="0" t="s">
         <v>151</v>
       </c>
       <c r="G1094" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="H1094" s="39"/>
+      <c r="H1094" s="38"/>
     </row>
     <row r="1095" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1095" s="0" t="s">
@@ -30041,14 +30040,14 @@
       </c>
     </row>
     <row r="1097" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1097" s="39"/>
+      <c r="B1097" s="38"/>
       <c r="F1097" s="0" t="s">
         <v>1321</v>
       </c>
       <c r="G1097" s="0" t="s">
         <v>1322</v>
       </c>
-      <c r="H1097" s="39"/>
+      <c r="H1097" s="38"/>
     </row>
     <row r="1098" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1098" s="0" t="s">
@@ -30084,14 +30083,14 @@
       </c>
     </row>
     <row r="1101" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1101" s="39"/>
+      <c r="B1101" s="38"/>
       <c r="F1101" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1101" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1101" s="39"/>
+      <c r="H1101" s="38"/>
     </row>
     <row r="1102" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1102" s="0" t="s">
@@ -30119,14 +30118,14 @@
       </c>
     </row>
     <row r="1104" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1104" s="39"/>
+      <c r="B1104" s="38"/>
       <c r="F1104" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1104" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1104" s="39"/>
+      <c r="H1104" s="38"/>
     </row>
     <row r="1105" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1105" s="0" t="s">
@@ -30154,14 +30153,14 @@
       </c>
     </row>
     <row r="1107" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1107" s="39"/>
+      <c r="B1107" s="38"/>
       <c r="F1107" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1107" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1107" s="39"/>
+      <c r="H1107" s="38"/>
     </row>
     <row r="1108" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1108" s="0" t="s">
@@ -30189,14 +30188,14 @@
       </c>
     </row>
     <row r="1110" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1110" s="39"/>
+      <c r="B1110" s="38"/>
       <c r="F1110" s="0" t="s">
         <v>159</v>
       </c>
       <c r="G1110" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1110" s="39"/>
+      <c r="H1110" s="38"/>
     </row>
     <row r="1111" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1111" s="0" t="s">
@@ -30224,7 +30223,7 @@
       </c>
     </row>
     <row r="1113" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1113" s="39"/>
+      <c r="B1113" s="38"/>
       <c r="D1113" s="5"/>
       <c r="E1113" s="5"/>
       <c r="F1113" s="0" t="s">
@@ -30233,7 +30232,7 @@
       <c r="G1113" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H1113" s="39"/>
+      <c r="H1113" s="38"/>
     </row>
     <row r="1114" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1114" s="0" t="s">
@@ -30689,7 +30688,7 @@
       <c r="H1142" s="0" t="s">
         <v>1377</v>
       </c>
-      <c r="I1142" s="36"/>
+      <c r="I1142" s="35"/>
       <c r="J1142" s="0" t="s">
         <v>45</v>
       </c>
@@ -30736,7 +30735,7 @@
       <c r="H1144" s="0" t="s">
         <v>1382</v>
       </c>
-      <c r="I1144" s="36"/>
+      <c r="I1144" s="35"/>
       <c r="J1144" s="0" t="s">
         <v>45</v>
       </c>
@@ -30774,7 +30773,7 @@
       <c r="E1146" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1146" s="36" t="s">
+      <c r="I1146" s="35" t="s">
         <v>789</v>
       </c>
       <c r="J1146" s="0" t="s">
@@ -30794,7 +30793,7 @@
       <c r="E1147" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1147" s="36" t="s">
+      <c r="I1147" s="35" t="s">
         <v>1387</v>
       </c>
       <c r="J1147" s="0" t="s">
@@ -30825,7 +30824,7 @@
       <c r="E1149" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1149" s="36" t="s">
+      <c r="I1149" s="35" t="s">
         <v>1387</v>
       </c>
       <c r="J1149" s="0" t="s">
@@ -30839,7 +30838,7 @@
       <c r="G1150" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="J1150" s="29"/>
+      <c r="J1150" s="28"/>
     </row>
     <row r="1151" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1151" s="0" t="s">
@@ -31522,7 +31521,7 @@
       <c r="E1200" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1200" s="29"/>
+      <c r="I1200" s="28"/>
       <c r="J1200" s="0" t="s">
         <v>21</v>
       </c>
@@ -31544,32 +31543,32 @@
       </c>
     </row>
     <row r="1203" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1203" s="29" t="s">
+      <c r="A1203" s="28" t="s">
         <v>1452</v>
       </c>
-      <c r="B1203" s="29" t="s">
+      <c r="B1203" s="28" t="s">
         <v>1453</v>
       </c>
-      <c r="C1203" s="29"/>
-      <c r="D1203" s="29" t="s">
+      <c r="C1203" s="28"/>
+      <c r="D1203" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="E1203" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1203" s="29"/>
-      <c r="G1203" s="29"/>
-      <c r="H1203" s="29"/>
-      <c r="J1203" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1203" s="29"/>
-      <c r="L1203" s="29"/>
-      <c r="M1203" s="29"/>
-      <c r="N1203" s="29"/>
-      <c r="O1203" s="29"/>
-      <c r="P1203" s="29"/>
-      <c r="Q1203" s="29"/>
+      <c r="E1203" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1203" s="28"/>
+      <c r="G1203" s="28"/>
+      <c r="H1203" s="28"/>
+      <c r="J1203" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1203" s="28"/>
+      <c r="L1203" s="28"/>
+      <c r="M1203" s="28"/>
+      <c r="N1203" s="28"/>
+      <c r="O1203" s="28"/>
+      <c r="P1203" s="28"/>
+      <c r="Q1203" s="28"/>
     </row>
     <row r="1204" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1204" s="0" t="s">
@@ -31771,7 +31770,7 @@
       <c r="L1221" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O1221" s="31" t="s">
+      <c r="O1221" s="30" t="s">
         <v>638</v>
       </c>
     </row>
@@ -31936,7 +31935,7 @@
       <c r="E1230" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1230" s="29"/>
+      <c r="I1230" s="28"/>
       <c r="J1230" s="0" t="s">
         <v>21</v>
       </c>
@@ -31958,36 +31957,36 @@
       </c>
     </row>
     <row r="1233" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1233" s="29" t="s">
+      <c r="A1233" s="28" t="s">
         <v>1485</v>
       </c>
-      <c r="B1233" s="29" t="s">
+      <c r="B1233" s="28" t="s">
         <v>1486</v>
       </c>
-      <c r="C1233" s="29"/>
-      <c r="D1233" s="29" t="s">
+      <c r="C1233" s="28"/>
+      <c r="D1233" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E1233" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1233" s="29"/>
-      <c r="G1233" s="29"/>
-      <c r="H1233" s="29" t="s">
+      <c r="E1233" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1233" s="28"/>
+      <c r="G1233" s="28"/>
+      <c r="H1233" s="28" t="s">
         <v>1487</v>
       </c>
-      <c r="J1233" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1233" s="29"/>
-      <c r="L1233" s="29"/>
-      <c r="M1233" s="29"/>
-      <c r="N1233" s="29"/>
-      <c r="O1233" s="29"/>
-      <c r="P1233" s="29" t="s">
+      <c r="J1233" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1233" s="28"/>
+      <c r="L1233" s="28"/>
+      <c r="M1233" s="28"/>
+      <c r="N1233" s="28"/>
+      <c r="O1233" s="28"/>
+      <c r="P1233" s="28" t="s">
         <v>1488</v>
       </c>
-      <c r="Q1233" s="29"/>
+      <c r="Q1233" s="28"/>
     </row>
     <row r="1234" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1234" s="0" t="s">
@@ -32896,7 +32895,7 @@
       <c r="L1303" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O1303" s="43" t="s">
+      <c r="O1303" s="42" t="s">
         <v>638</v>
       </c>
     </row>
@@ -32942,7 +32941,7 @@
       <c r="L1305" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O1305" s="43" t="s">
+      <c r="O1305" s="42" t="s">
         <v>638</v>
       </c>
     </row>
@@ -33110,7 +33109,7 @@
       <c r="L1317" s="0" t="s">
         <v>637</v>
       </c>
-      <c r="O1317" s="44" t="s">
+      <c r="O1317" s="43" t="s">
         <v>638</v>
       </c>
     </row>
@@ -33599,7 +33598,7 @@
       <c r="E1356" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="I1356" s="34"/>
+      <c r="I1356" s="33"/>
       <c r="J1356" s="0" t="s">
         <v>45</v>
       </c>
@@ -33619,7 +33618,7 @@
       <c r="G1358" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="I1358" s="34"/>
+      <c r="I1358" s="33"/>
     </row>
     <row r="1359" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1359" s="0" t="s">
@@ -33634,7 +33633,7 @@
       <c r="E1359" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1359" s="34"/>
+      <c r="G1359" s="33"/>
       <c r="J1359" s="0" t="s">
         <v>45</v>
       </c>
@@ -33646,13 +33645,13 @@
       <c r="G1360" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="I1360" s="34"/>
+      <c r="I1360" s="33"/>
     </row>
     <row r="1361" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1361" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G1361" s="34" t="s">
+      <c r="G1361" s="33" t="s">
         <v>45</v>
       </c>
     </row>
@@ -33677,7 +33676,7 @@
       <c r="F1363" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G1363" s="34" t="s">
+      <c r="G1363" s="33" t="s">
         <v>21</v>
       </c>
     </row>
@@ -33702,7 +33701,7 @@
       <c r="E1365" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1365" s="34"/>
+      <c r="G1365" s="33"/>
       <c r="J1365" s="0" t="s">
         <v>45</v>
       </c>
@@ -33711,7 +33710,7 @@
       <c r="F1366" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="G1366" s="34" t="s">
+      <c r="G1366" s="33" t="s">
         <v>21</v>
       </c>
     </row>
@@ -33719,7 +33718,7 @@
       <c r="F1367" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G1367" s="34" t="s">
+      <c r="G1367" s="33" t="s">
         <v>45</v>
       </c>
     </row>
@@ -33736,7 +33735,7 @@
       <c r="E1368" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="G1368" s="34"/>
+      <c r="G1368" s="33"/>
       <c r="J1368" s="0" t="s">
         <v>21</v>
       </c>
@@ -33754,7 +33753,7 @@
       <c r="E1369" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="G1369" s="34"/>
+      <c r="G1369" s="33"/>
       <c r="J1369" s="0" t="s">
         <v>21</v>
       </c>
@@ -33772,7 +33771,7 @@
       <c r="E1370" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="G1370" s="34"/>
+      <c r="G1370" s="33"/>
       <c r="J1370" s="0" t="s">
         <v>21</v>
       </c>
@@ -33790,7 +33789,7 @@
       <c r="E1371" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1371" s="34"/>
+      <c r="G1371" s="33"/>
       <c r="H1371" s="0" t="s">
         <v>1646</v>
       </c>
@@ -33814,7 +33813,7 @@
       <c r="E1372" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1372" s="34"/>
+      <c r="G1372" s="33"/>
       <c r="H1372" s="0" t="s">
         <v>1649</v>
       </c>
@@ -33838,7 +33837,7 @@
       <c r="E1373" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1373" s="34"/>
+      <c r="G1373" s="33"/>
       <c r="H1373" s="0" t="s">
         <v>1653</v>
       </c>
@@ -33862,7 +33861,7 @@
       <c r="E1374" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1374" s="34"/>
+      <c r="G1374" s="33"/>
       <c r="J1374" s="0" t="s">
         <v>21</v>
       </c>
@@ -33874,13 +33873,13 @@
       <c r="G1375" s="0" t="s">
         <v>1658</v>
       </c>
-      <c r="H1375" s="34"/>
+      <c r="H1375" s="33"/>
     </row>
     <row r="1376" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="F1376" s="0" t="s">
         <v>1659</v>
       </c>
-      <c r="G1376" s="34" t="s">
+      <c r="G1376" s="33" t="s">
         <v>1660</v>
       </c>
     </row>
@@ -33897,7 +33896,7 @@
       <c r="E1377" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1377" s="34"/>
+      <c r="G1377" s="33"/>
       <c r="H1377" s="0" t="s">
         <v>1663</v>
       </c>
@@ -33921,7 +33920,7 @@
       <c r="E1378" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1378" s="34"/>
+      <c r="G1378" s="33"/>
       <c r="H1378" s="0" t="s">
         <v>34</v>
       </c>
@@ -33936,7 +33935,7 @@
       <c r="F1379" s="0" t="s">
         <v>1387</v>
       </c>
-      <c r="G1379" s="34" t="s">
+      <c r="G1379" s="33" t="s">
         <v>1667</v>
       </c>
     </row>
@@ -33956,7 +33955,7 @@
       <c r="H1380" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="I1380" s="36" t="s">
+      <c r="I1380" s="35" t="s">
         <v>1387</v>
       </c>
       <c r="J1380" s="0" t="s">
@@ -33984,7 +33983,7 @@
       <c r="E1382" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1382" s="34"/>
+      <c r="G1382" s="33"/>
       <c r="H1382" s="0" t="s">
         <v>34</v>
       </c>
@@ -33999,7 +33998,7 @@
       <c r="F1383" s="0" t="s">
         <v>1387</v>
       </c>
-      <c r="G1383" s="34" t="s">
+      <c r="G1383" s="33" t="s">
         <v>1667</v>
       </c>
     </row>
@@ -34016,7 +34015,7 @@
       <c r="E1384" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1384" s="34"/>
+      <c r="G1384" s="33"/>
       <c r="H1384" s="0" t="s">
         <v>34</v>
       </c>
@@ -34031,7 +34030,7 @@
       <c r="F1385" s="0" t="s">
         <v>373</v>
       </c>
-      <c r="G1385" s="34" t="s">
+      <c r="G1385" s="33" t="s">
         <v>374</v>
       </c>
     </row>
@@ -34039,7 +34038,7 @@
       <c r="F1386" s="0" t="s">
         <v>1673</v>
       </c>
-      <c r="G1386" s="34" t="s">
+      <c r="G1386" s="33" t="s">
         <v>1674</v>
       </c>
     </row>
@@ -34047,7 +34046,7 @@
       <c r="F1387" s="0" t="s">
         <v>1675</v>
       </c>
-      <c r="G1387" s="34" t="s">
+      <c r="G1387" s="33" t="s">
         <v>1676</v>
       </c>
     </row>
@@ -34055,7 +34054,7 @@
       <c r="F1388" s="0" t="s">
         <v>1677</v>
       </c>
-      <c r="G1388" s="34" t="s">
+      <c r="G1388" s="33" t="s">
         <v>1678</v>
       </c>
     </row>
@@ -34063,7 +34062,7 @@
       <c r="F1389" s="0" t="s">
         <v>1679</v>
       </c>
-      <c r="G1389" s="34" t="s">
+      <c r="G1389" s="33" t="s">
         <v>1680</v>
       </c>
     </row>
@@ -34071,7 +34070,7 @@
       <c r="F1390" s="0" t="s">
         <v>1681</v>
       </c>
-      <c r="G1390" s="34" t="s">
+      <c r="G1390" s="33" t="s">
         <v>1682</v>
       </c>
     </row>
@@ -34800,7 +34799,7 @@
       <c r="H1444" s="0" t="s">
         <v>1738</v>
       </c>
-      <c r="I1444" s="34"/>
+      <c r="I1444" s="33"/>
       <c r="J1444" s="0" t="s">
         <v>21</v>
       </c>
@@ -34847,7 +34846,7 @@
       <c r="H1446" s="0" t="s">
         <v>1743</v>
       </c>
-      <c r="I1446" s="34"/>
+      <c r="I1446" s="33"/>
       <c r="J1446" s="0" t="s">
         <v>21</v>
       </c>
@@ -34891,11 +34890,11 @@
       <c r="E1448" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1448" s="34"/>
+      <c r="G1448" s="33"/>
       <c r="H1448" s="0" t="s">
         <v>1748</v>
       </c>
-      <c r="I1448" s="34"/>
+      <c r="I1448" s="33"/>
       <c r="J1448" s="0" t="s">
         <v>21</v>
       </c>
@@ -34939,7 +34938,7 @@
       <c r="E1450" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G1450" s="34"/>
+      <c r="G1450" s="33"/>
       <c r="H1450" s="0" t="s">
         <v>1753</v>
       </c>
@@ -34986,7 +34985,7 @@
       <c r="E1452" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G1452" s="34"/>
+      <c r="G1452" s="33"/>
       <c r="H1452" s="0" t="s">
         <v>1757</v>
       </c>
@@ -35372,7 +35371,7 @@
       <c r="E1472" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1472" s="34"/>
+      <c r="G1472" s="33"/>
       <c r="H1472" s="0" t="s">
         <v>34</v>
       </c>
@@ -35387,7 +35386,7 @@
       <c r="F1473" s="0" t="s">
         <v>357</v>
       </c>
-      <c r="G1473" s="34" t="s">
+      <c r="G1473" s="33" t="s">
         <v>358</v>
       </c>
     </row>
@@ -35404,7 +35403,7 @@
       <c r="E1474" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="G1474" s="34"/>
+      <c r="G1474" s="33"/>
       <c r="H1474" s="0" t="s">
         <v>34</v>
       </c>
@@ -35419,7 +35418,7 @@
       <c r="F1475" s="0" t="s">
         <v>398</v>
       </c>
-      <c r="G1475" s="34" t="s">
+      <c r="G1475" s="33" t="s">
         <v>399</v>
       </c>
     </row>
@@ -35490,7 +35489,7 @@
       <c r="F1482" s="0" t="s">
         <v>1797</v>
       </c>
-      <c r="G1482" s="35" t="s">
+      <c r="G1482" s="34" t="s">
         <v>1798</v>
       </c>
     </row>
@@ -35498,7 +35497,7 @@
       <c r="F1483" s="0" t="s">
         <v>1799</v>
       </c>
-      <c r="G1483" s="35" t="s">
+      <c r="G1483" s="34" t="s">
         <v>1800</v>
       </c>
     </row>
@@ -35506,7 +35505,7 @@
       <c r="F1484" s="0" t="s">
         <v>1801</v>
       </c>
-      <c r="G1484" s="35" t="s">
+      <c r="G1484" s="34" t="s">
         <v>1802</v>
       </c>
     </row>
@@ -35514,7 +35513,7 @@
       <c r="F1485" s="0" t="s">
         <v>1803</v>
       </c>
-      <c r="G1485" s="35" t="s">
+      <c r="G1485" s="34" t="s">
         <v>1804</v>
       </c>
     </row>
@@ -35522,7 +35521,7 @@
       <c r="F1486" s="0" t="s">
         <v>1805</v>
       </c>
-      <c r="G1486" s="35" t="s">
+      <c r="G1486" s="34" t="s">
         <v>1806</v>
       </c>
     </row>
@@ -35553,7 +35552,7 @@
       <c r="F1488" s="0" t="s">
         <v>1082</v>
       </c>
-      <c r="G1488" s="35" t="s">
+      <c r="G1488" s="34" t="s">
         <v>1083</v>
       </c>
     </row>
@@ -35561,7 +35560,7 @@
       <c r="F1489" s="0" t="s">
         <v>1088</v>
       </c>
-      <c r="G1489" s="35" t="s">
+      <c r="G1489" s="34" t="s">
         <v>1089</v>
       </c>
     </row>
@@ -35569,7 +35568,7 @@
       <c r="F1490" s="0" t="s">
         <v>1092</v>
       </c>
-      <c r="G1490" s="35" t="s">
+      <c r="G1490" s="34" t="s">
         <v>1093</v>
       </c>
     </row>
@@ -35983,7 +35982,7 @@
   <conditionalFormatting sqref="A159:A558">
     <cfRule type="duplicateValues" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0"/>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="J2:J31 J33:J54 J57:J58 J61:J62 J65:J158" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
@@ -35992,8 +35991,12 @@
       <formula1>INDIRECT(D128)</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E31 E33:E54 E57:E58 E61:E62 E65:E126 E129:E158 E1020:E1026 E1030 E1034:E1039 E1049 E1062:E1067 E1077:E1081 E1100 E1113" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E2:E31 E33:E54 E57:E58 E61:E62 E65:E126 E129:E158 E1020:E1026 E1030 E1034:E1039 E1049 E1062:E1067 E1077:E1080 E1100 E1113" type="list">
       <formula1>INDIRECT(D61)</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="E1081" type="list">
+      <formula1>INDIRECT(D1140)</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>